<commit_message>
Working on truth state and continuous measurement
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="257">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -228,7 +228,7 @@
     <t xml:space="preserve">Gyro bias ECRV time constant</t>
   </si>
   <si>
-    <t xml:space="preserve">tau_st</t>
+    <t xml:space="preserve">tau_b</t>
   </si>
   <si>
     <t xml:space="preserve">Camera misalignment ECRV time constant</t>
@@ -354,6 +354,24 @@
     <t xml:space="preserve">Initial launch angle</t>
   </si>
   <si>
+    <t xml:space="preserve">u_beta_x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X component of lunar lander rotation axis (inertial frame)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u_beta_y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y component of lunar lander rotation axis (inertial frame)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u_beta_z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z component of lunar lander rotation axis (inertial frame)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ri_x</t>
   </si>
   <si>
@@ -513,7 +531,7 @@
     <t xml:space="preserve">vel</t>
   </si>
   <si>
-    <t xml:space="preserve">cam_att_disp</t>
+    <t xml:space="preserve">cam</t>
   </si>
   <si>
     <t xml:space="preserve">acc_bias</t>
@@ -1324,7 +1342,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A2:A22"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="A39:E41 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1512,8 +1530,8 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A39:E41 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1545,7 +1563,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="61" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B2" s="33" t="n">
         <v>0.1</v>
@@ -1554,7 +1572,7 @@
         <v>55</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E2" s="34" t="n">
         <f aca="false">B2</f>
@@ -1564,7 +1582,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="61" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B3" s="33" t="n">
         <v>0.2</v>
@@ -1573,7 +1591,7 @@
         <v>55</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E3" s="34" t="n">
         <f aca="false">B3</f>
@@ -1583,7 +1601,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="61" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B4" s="33" t="n">
         <v>0.3</v>
@@ -1592,7 +1610,7 @@
         <v>55</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E4" s="39" t="n">
         <f aca="false">B4</f>
@@ -1602,16 +1620,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="61" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B5" s="36" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E5" s="34" t="n">
         <f aca="false">B5</f>
@@ -1621,16 +1639,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="61" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B6" s="36" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E6" s="34" t="n">
         <f aca="false">B6</f>
@@ -1640,16 +1658,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="61" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B7" s="36" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E7" s="34" t="n">
         <f aca="false">B7</f>
@@ -1659,7 +1677,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="61" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B8" s="40" t="n">
         <v>0.1</v>
@@ -1668,7 +1686,7 @@
         <v>68</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E8" s="42" t="n">
         <f aca="false">RADIANS(B8)</f>
@@ -1678,7 +1696,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="61" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B9" s="43" t="n">
         <v>0.2</v>
@@ -1687,7 +1705,7 @@
         <v>68</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E9" s="44" t="n">
         <f aca="false">RADIANS(B9)</f>
@@ -1697,7 +1715,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="61" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B10" s="43" t="n">
         <v>0.3</v>
@@ -1706,7 +1724,7 @@
         <v>68</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E10" s="46" t="n">
         <f aca="false">RADIANS(B10)</f>
@@ -1716,16 +1734,16 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="61" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="B11" s="47" t="n">
         <v>0.1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E11" s="48" t="n">
         <f aca="false">B11</f>
@@ -1735,16 +1753,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="61" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B12" s="49" t="n">
         <v>0.1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="E12" s="50" t="n">
         <f aca="false">B12</f>
@@ -1754,16 +1772,16 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="61" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B13" s="49" t="n">
         <v>0.1</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E13" s="51" t="n">
         <f aca="false">B13</f>
@@ -1773,7 +1791,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="61" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>0.1</v>
@@ -1782,7 +1800,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E14" s="52" t="n">
         <f aca="false">B14</f>
@@ -1792,7 +1810,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="61" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>0.2</v>
@@ -1801,7 +1819,7 @@
         <v>55</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E15" s="53" t="n">
         <f aca="false">B15</f>
@@ -1811,7 +1829,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="61" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B16" s="33" t="n">
         <v>0.3</v>
@@ -1820,7 +1838,7 @@
         <v>55</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">B16</f>
@@ -1830,7 +1848,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="61" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B17" s="33" t="n">
         <v>0.1</v>
@@ -1839,7 +1857,7 @@
         <v>55</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E17" s="52" t="n">
         <f aca="false">B17</f>
@@ -1849,7 +1867,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="61" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B18" s="33" t="n">
         <v>0.2</v>
@@ -1858,7 +1876,7 @@
         <v>55</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E18" s="53" t="n">
         <f aca="false">B18</f>
@@ -1868,7 +1886,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="61" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B19" s="33" t="n">
         <v>0.3</v>
@@ -1877,7 +1895,7 @@
         <v>55</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">B19</f>
@@ -1887,7 +1905,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="61" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B20" s="33" t="n">
         <v>0.1</v>
@@ -1896,7 +1914,7 @@
         <v>55</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E20" s="52" t="n">
         <f aca="false">B20</f>
@@ -1905,7 +1923,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="61" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B21" s="33" t="n">
         <v>0.2</v>
@@ -1914,7 +1932,7 @@
         <v>55</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E21" s="53" t="n">
         <f aca="false">B21</f>
@@ -1923,7 +1941,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="61" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B22" s="33" t="n">
         <v>0.3</v>
@@ -1932,7 +1950,7 @@
         <v>55</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">B22</f>
@@ -1958,7 +1976,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A2:A22"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="A39:E41 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1970,7 +1988,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>60</v>
@@ -1978,7 +1996,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>60</v>
@@ -1986,7 +2004,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">hr2min*min2sec</f>
@@ -1995,7 +2013,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>9.81</v>
@@ -2003,7 +2021,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>24</v>
@@ -2011,7 +2029,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">180/3.14159</f>
@@ -2036,8 +2054,8 @@
   </sheetPr>
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="1" sqref="A2:A22 D30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2741,16 +2759,58 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0"/>
-      <c r="E39" s="0"/>
+      <c r="A39" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" s="16" t="n">
+        <f aca="false">B39</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0"/>
-      <c r="E40" s="0"/>
+      <c r="A40" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="16" t="n">
+        <f aca="false">B40</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0"/>
-      <c r="E41" s="0"/>
+      <c r="A41" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="16" t="n">
+        <f aca="false">B41</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0"/>
@@ -2775,7 +2835,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="1" sqref="A2:A22 B24"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A39:E41 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2805,7 +2865,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" s="33" t="n">
         <v>1737</v>
@@ -2814,7 +2874,7 @@
         <v>43</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E2" s="34" t="n">
         <f aca="false">B2*1000</f>
@@ -2823,7 +2883,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="35" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B3" s="36" t="n">
         <v>0</v>
@@ -2832,7 +2892,7 @@
         <v>43</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E3" s="34" t="n">
         <f aca="false">B3*1000</f>
@@ -2841,7 +2901,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="37" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B4" s="38" t="n">
         <v>0</v>
@@ -2850,7 +2910,7 @@
         <v>43</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E4" s="39" t="n">
         <f aca="false">B4*1000</f>
@@ -2859,16 +2919,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B5" s="36" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>112</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>106</v>
       </c>
       <c r="E5" s="34" t="n">
         <f aca="false">B5*1000</f>
@@ -2877,16 +2937,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B6" s="36" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E6" s="34" t="n">
         <f aca="false">B6*1000</f>
@@ -2895,16 +2955,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="35" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B7" s="36" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E7" s="34" t="n">
         <f aca="false">B7*1000</f>
@@ -2913,7 +2973,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B8" s="40" t="n">
         <v>1</v>
@@ -2922,7 +2982,7 @@
         <v>68</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E8" s="42" t="n">
         <f aca="false">RADIANS(B8)</f>
@@ -2931,7 +2991,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B9" s="43" t="n">
         <v>1</v>
@@ -2940,7 +3000,7 @@
         <v>68</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E9" s="44" t="n">
         <f aca="false">RADIANS(B9)</f>
@@ -2949,7 +3009,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="45" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B10" s="43" t="n">
         <v>1</v>
@@ -2958,7 +3018,7 @@
         <v>68</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E10" s="46" t="n">
         <f aca="false">RADIANS(B10)</f>
@@ -2967,16 +3027,16 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B11" s="47" t="n">
         <v>0.1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E11" s="48" t="n">
         <f aca="false">B11</f>
@@ -2985,16 +3045,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B12" s="49" t="n">
         <v>0.1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="E12" s="50" t="n">
         <f aca="false">B12</f>
@@ -3003,16 +3063,16 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B13" s="49" t="n">
         <v>0.1</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E13" s="51" t="n">
         <f aca="false">B13</f>
@@ -3021,7 +3081,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>1737</v>
@@ -3030,7 +3090,7 @@
         <v>43</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E14" s="52" t="n">
         <f aca="false">B14*1000</f>
@@ -3039,7 +3099,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B15" s="36" t="n">
         <v>0.001</v>
@@ -3048,7 +3108,7 @@
         <v>43</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E15" s="53" t="n">
         <f aca="false">B15*1000</f>
@@ -3057,7 +3117,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B16" s="38" t="n">
         <v>0</v>
@@ -3066,7 +3126,7 @@
         <v>43</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">B16*1000</f>
@@ -3075,7 +3135,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B17" s="33" t="n">
         <v>1737</v>
@@ -3084,7 +3144,7 @@
         <v>43</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E17" s="52" t="n">
         <f aca="false">B17*1000</f>
@@ -3093,7 +3153,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B18" s="36" t="n">
         <v>0</v>
@@ -3102,7 +3162,7 @@
         <v>43</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E18" s="53" t="n">
         <f aca="false">B18*1000</f>
@@ -3111,7 +3171,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B19" s="38" t="n">
         <v>0.001</v>
@@ -3120,7 +3180,7 @@
         <v>43</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">B19*1000</f>
@@ -3129,7 +3189,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B20" s="33" t="n">
         <v>1737</v>
@@ -3138,7 +3198,7 @@
         <v>43</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E20" s="52" t="n">
         <f aca="false">B20*1000</f>
@@ -3147,7 +3207,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B21" s="36" t="n">
         <v>0.001</v>
@@ -3156,7 +3216,7 @@
         <v>43</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E21" s="53" t="n">
         <f aca="false">B21*1000</f>
@@ -3165,7 +3225,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B22" s="38" t="n">
         <v>0.001</v>
@@ -3174,7 +3234,7 @@
         <v>43</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">B22*1000</f>
@@ -3183,7 +3243,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="35" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B23" s="35" t="n">
         <v>1</v>
@@ -3192,7 +3252,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E23" s="55" t="n">
         <f aca="false">B23</f>
@@ -3201,7 +3261,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="35" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B24" s="35" t="n">
         <v>0</v>
@@ -3210,7 +3270,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E24" s="8" t="n">
         <f aca="false">B24/3</f>
@@ -3219,7 +3279,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="35" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B25" s="35" t="n">
         <v>0</v>
@@ -3228,7 +3288,7 @@
         <v>6</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E25" s="55" t="n">
         <f aca="false">B25/3</f>
@@ -3237,7 +3297,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="35" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B26" s="35" t="n">
         <v>0</v>
@@ -3246,7 +3306,7 @@
         <v>6</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E26" s="55" t="n">
         <f aca="false">B26/3</f>
@@ -3272,7 +3332,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="1" sqref="A2:A22 D13"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="A39:E41 A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3285,24 +3345,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -3319,7 +3379,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
@@ -3336,7 +3396,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>7</v>
@@ -3353,7 +3413,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>10</v>
@@ -3370,7 +3430,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>13</v>
@@ -3387,7 +3447,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>16</v>
@@ -3404,7 +3464,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>19</v>
@@ -3421,7 +3481,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>22</v>
@@ -3438,7 +3498,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B2</f>
@@ -3480,7 +3540,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">B9</f>
@@ -3501,7 +3561,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">B2</f>
@@ -3539,7 +3599,7 @@
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="1" sqref="A2:A22 E11"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A39:E41 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3552,24 +3612,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -3586,7 +3646,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
@@ -3603,7 +3663,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>7</v>
@@ -3620,7 +3680,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>10</v>
@@ -3637,7 +3697,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>13</v>
@@ -3654,7 +3714,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>16</v>
@@ -3671,7 +3731,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>19</v>
@@ -3688,7 +3748,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B2</f>
@@ -3730,7 +3790,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B2</f>
@@ -4729,7 +4789,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A22 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A39:E41 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4762,17 +4822,17 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="61" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B2" s="62" t="n">
         <f aca="false">0.00000016*3</f>
         <v>4.8E-007</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E2" s="44" t="n">
         <f aca="false">B2/3</f>
@@ -4781,16 +4841,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="61" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B3" s="63" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="E3" s="44" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
@@ -4800,16 +4860,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B4" s="64" t="n">
         <v>0.05</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="E4" s="46" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
@@ -4818,16 +4878,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="61" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B5" s="63" t="n">
         <v>20</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="E5" s="44" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
@@ -4836,16 +4896,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="61" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B6" s="63" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E6" s="44" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
@@ -4854,16 +4914,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B7" s="63" t="n">
         <v>1.5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E7" s="44" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
@@ -4872,16 +4932,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B8" s="63" t="n">
         <v>1.5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E8" s="44" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
@@ -4890,16 +4950,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B9" s="63" t="n">
         <v>9</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E9" s="44" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
@@ -4908,16 +4968,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B10" s="40" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="E10" s="42" t="n">
         <f aca="false">B10/3</f>
@@ -4926,16 +4986,16 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="45" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B11" s="65" t="n">
         <v>3</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E11" s="46" t="n">
         <f aca="false">B11/3</f>
@@ -4944,7 +5004,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B12" s="56" t="n">
         <v>10</v>
@@ -4953,7 +5013,7 @@
         <v>55</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E12" s="10" t="n">
         <f aca="false">B12/3</f>
@@ -4962,7 +5022,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B13" s="56" t="n">
         <v>100</v>
@@ -4971,7 +5031,7 @@
         <v>55</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E13" s="10" t="n">
         <f aca="false">B13/3</f>
@@ -4980,7 +5040,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B14" s="56" t="n">
         <v>10</v>
@@ -4989,7 +5049,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="E14" s="10" t="n">
         <f aca="false">B14/3</f>
@@ -5015,7 +5075,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A2:A22 B19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A39:E41 B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5047,7 +5107,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="67" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B2" s="41" t="n">
         <v>4000</v>
@@ -5056,7 +5116,7 @@
         <v>55</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E2" s="42" t="n">
         <f aca="false">B2/3</f>
@@ -5065,7 +5125,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="61" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B3" s="35" t="n">
         <v>4000</v>
@@ -5074,7 +5134,7 @@
         <v>55</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E3" s="44" t="n">
         <f aca="false">B3/3</f>
@@ -5083,7 +5143,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="61" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B4" s="35" t="n">
         <v>4000</v>
@@ -5092,7 +5152,7 @@
         <v>55</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E4" s="44" t="n">
         <f aca="false">B4/3</f>
@@ -5101,16 +5161,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="61" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B5" s="35" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E5" s="44" t="n">
         <f aca="false">B5/3</f>
@@ -5119,16 +5179,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="61" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B6" s="35" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E6" s="44" t="n">
         <f aca="false">B6/3</f>
@@ -5137,16 +5197,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="61" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B7" s="35" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E7" s="44" t="n">
         <f aca="false">B7/3</f>
@@ -5155,16 +5215,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="61" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B8" s="35" t="n">
         <v>0.0005</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="E8" s="44" t="n">
         <f aca="false">B8/3</f>
@@ -5173,16 +5233,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="61" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B9" s="35" t="n">
         <v>0.0005</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="E9" s="44" t="n">
         <f aca="false">B9/3</f>
@@ -5191,16 +5251,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="61" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B10" s="35" t="n">
         <v>0.0005</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="E10" s="44" t="n">
         <f aca="false">B10/3</f>
@@ -5209,17 +5269,17 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="61" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B11" s="35" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E11" s="44" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
@@ -5228,17 +5288,17 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B12" s="35" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E12" s="44" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
@@ -5247,17 +5307,17 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B13" s="35" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E13" s="44" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
@@ -5266,17 +5326,17 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B14" s="35" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="E14" s="44" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
@@ -5285,17 +5345,17 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B15" s="35" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="E15" s="44" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
@@ -5304,17 +5364,17 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B16" s="35" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="E16" s="44" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
@@ -5323,17 +5383,17 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="61" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B17" s="35" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C17" s="62" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="E17" s="44" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
@@ -5342,17 +5402,17 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="61" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B18" s="35" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C18" s="62" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="E18" s="44" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
@@ -5361,17 +5421,17 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B19" s="37" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C19" s="68" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="E19" s="46" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
@@ -5397,7 +5457,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A22 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A39:E41 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5737,7 +5797,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A2:A22 B19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A39:E41 B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
truth diffeq doing good work
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -348,7 +348,7 @@
     <t xml:space="preserve">Thrust to weight ratio of the ship</t>
   </si>
   <si>
-    <t xml:space="preserve">beta</t>
+    <t xml:space="preserve">b</t>
   </si>
   <si>
     <t xml:space="preserve">Initial launch angle</t>
@@ -981,7 +981,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1094,22 +1094,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1122,15 +1106,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1146,27 +1122,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1175,10 +1131,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1202,10 +1154,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1226,18 +1174,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1247,10 +1183,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1342,14 +1274,14 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="A39:E41 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,7 +1463,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A39:E41 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1540,203 +1472,203 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="8" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="69" t="s">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="47" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="33" t="n">
+      <c r="B2" s="29" t="n">
         <v>0.1</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="34" t="n">
+      <c r="E2" s="30" t="n">
         <f aca="false">B2</f>
         <v>0.1</v>
       </c>
-      <c r="F2" s="35"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="33" t="n">
+      <c r="B3" s="29" t="n">
         <v>0.2</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="34" t="n">
+      <c r="E3" s="30" t="n">
         <f aca="false">B3</f>
         <v>0.2</v>
       </c>
-      <c r="F3" s="35"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B4" s="33" t="n">
+      <c r="B4" s="29" t="n">
         <v>0.3</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E4" s="39" t="n">
+      <c r="E4" s="33" t="n">
         <f aca="false">B4</f>
         <v>0.3</v>
       </c>
-      <c r="F4" s="35"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="B5" s="36" t="n">
+      <c r="B5" s="31" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="34" t="n">
+      <c r="E5" s="30" t="n">
         <f aca="false">B5</f>
         <v>1</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="B6" s="36" t="n">
+      <c r="B6" s="31" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="34" t="n">
+      <c r="E6" s="30" t="n">
         <f aca="false">B6</f>
         <v>2</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B7" s="36" t="n">
+      <c r="B7" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="34" t="n">
+      <c r="E7" s="30" t="n">
         <f aca="false">B7</f>
         <v>3</v>
       </c>
-      <c r="F7" s="35"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="34" t="n">
         <v>0.1</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="E8" s="42" t="n">
+      <c r="E8" s="14" t="n">
         <f aca="false">RADIANS(B8)</f>
         <v>0.00174532925199433</v>
       </c>
-      <c r="F8" s="35"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B9" s="43" t="n">
+      <c r="B9" s="35" t="n">
         <v>0.2</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E9" s="44" t="n">
+      <c r="E9" s="16" t="n">
         <f aca="false">RADIANS(B9)</f>
         <v>0.00349065850398866</v>
       </c>
-      <c r="F9" s="35"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B10" s="43" t="n">
+      <c r="B10" s="35" t="n">
         <v>0.3</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="46" t="n">
+      <c r="E10" s="27" t="n">
         <f aca="false">RADIANS(B10)</f>
         <v>0.00523598775598299</v>
       </c>
-      <c r="F10" s="35"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="B11" s="47" t="n">
+      <c r="B11" s="36" t="n">
         <v>0.1</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -1745,17 +1677,17 @@
       <c r="D11" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="E11" s="48" t="n">
+      <c r="E11" s="37" t="n">
         <f aca="false">B11</f>
         <v>0.1</v>
       </c>
-      <c r="F11" s="35"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="B12" s="49" t="n">
+      <c r="B12" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -1764,195 +1696,195 @@
       <c r="D12" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E12" s="50" t="n">
+      <c r="E12" s="38" t="n">
         <f aca="false">B12</f>
         <v>0.1</v>
       </c>
-      <c r="F12" s="35"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="B13" s="49" t="n">
+      <c r="B13" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="51" t="n">
+      <c r="E13" s="39" t="n">
         <f aca="false">B13</f>
         <v>0.1</v>
       </c>
-      <c r="F13" s="35"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B14" s="33" t="n">
+      <c r="B14" s="29" t="n">
         <v>0.1</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="52" t="n">
+      <c r="E14" s="40" t="n">
         <f aca="false">B14</f>
         <v>0.1</v>
       </c>
-      <c r="F14" s="35"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="B15" s="33" t="n">
+      <c r="B15" s="29" t="n">
         <v>0.2</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E15" s="53" t="n">
+      <c r="E15" s="41" t="n">
         <f aca="false">B15</f>
         <v>0.2</v>
       </c>
-      <c r="F15" s="35"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B16" s="33" t="n">
+      <c r="B16" s="29" t="n">
         <v>0.3</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="E16" s="54" t="n">
+      <c r="E16" s="42" t="n">
         <f aca="false">B16</f>
         <v>0.3</v>
       </c>
-      <c r="F16" s="35"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B17" s="33" t="n">
+      <c r="B17" s="29" t="n">
         <v>0.1</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="E17" s="52" t="n">
+      <c r="E17" s="40" t="n">
         <f aca="false">B17</f>
         <v>0.1</v>
       </c>
-      <c r="F17" s="35"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B18" s="33" t="n">
+      <c r="B18" s="29" t="n">
         <v>0.2</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E18" s="53" t="n">
+      <c r="E18" s="41" t="n">
         <f aca="false">B18</f>
         <v>0.2</v>
       </c>
-      <c r="F18" s="35"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B19" s="33" t="n">
+      <c r="B19" s="29" t="n">
         <v>0.3</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="E19" s="54" t="n">
+      <c r="E19" s="42" t="n">
         <f aca="false">B19</f>
         <v>0.3</v>
       </c>
-      <c r="F19" s="37"/>
+      <c r="F19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="B20" s="33" t="n">
+      <c r="B20" s="29" t="n">
         <v>0.1</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="E20" s="52" t="n">
+      <c r="E20" s="40" t="n">
         <f aca="false">B20</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="61" t="s">
+      <c r="A21" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B21" s="33" t="n">
+      <c r="B21" s="29" t="n">
         <v>0.2</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E21" s="53" t="n">
+      <c r="E21" s="41" t="n">
         <f aca="false">B21</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B22" s="33" t="n">
+      <c r="B22" s="29" t="n">
         <v>0.3</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="54" t="n">
+      <c r="E22" s="42" t="n">
         <f aca="false">B22</f>
         <v>0.3</v>
       </c>
@@ -1976,7 +1908,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="A39:E41 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2055,12 +1987,12 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39:E41"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="75.57"/>
@@ -2127,8 +2059,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="15" t="n">
-        <f aca="false">B5*0.5</f>
-        <v>3404.71010099543</v>
+        <v>10000</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>23</v>
@@ -2138,7 +2069,7 @@
       </c>
       <c r="E4" s="16" t="n">
         <f aca="false">B4</f>
-        <v>3404.71010099543</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,7 +2676,7 @@
         <v>103</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>0.005</v>
+        <v>0.05</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>68</v>
@@ -2755,7 +2686,7 @@
       </c>
       <c r="E38" s="0" t="n">
         <f aca="false">RADIANS(B38)</f>
-        <v>8.72664625997165E-005</v>
+        <v>0.000872664625997165</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2781,7 +2712,7 @@
         <v>107</v>
       </c>
       <c r="B40" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>55</v>
@@ -2791,7 +2722,7 @@
       </c>
       <c r="E40" s="16" t="n">
         <f aca="false">B40</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2799,7 +2730,7 @@
         <v>109</v>
       </c>
       <c r="B41" s="15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>55</v>
@@ -2809,7 +2740,7 @@
       </c>
       <c r="E41" s="16" t="n">
         <f aca="false">B41</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,7 +2766,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A39:E41 A2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2847,72 +2778,72 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="33" t="n">
+      <c r="B2" s="29" t="n">
         <v>1737</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="34" t="n">
+      <c r="E2" s="30" t="n">
         <f aca="false">B2*1000</f>
         <v>1737000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="35" t="s">
+      <c r="B3" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="34" t="n">
+      <c r="E3" s="30" t="n">
         <f aca="false">B3*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="37" t="s">
+      <c r="B4" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E4" s="39" t="n">
+      <c r="E4" s="33" t="n">
         <f aca="false">B4*1000</f>
         <v>0</v>
       </c>
@@ -2921,16 +2852,16 @@
       <c r="A5" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="36" t="n">
+      <c r="B5" s="31" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="34" t="n">
+      <c r="E5" s="30" t="n">
         <f aca="false">B5*1000</f>
         <v>0</v>
       </c>
@@ -2939,34 +2870,34 @@
       <c r="A6" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="36" t="n">
+      <c r="B6" s="31" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="34" t="n">
+      <c r="E6" s="30" t="n">
         <f aca="false">B6*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="35" t="s">
+      <c r="B7" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="34" t="n">
+      <c r="E7" s="30" t="n">
         <f aca="false">B7*1000</f>
         <v>0</v>
       </c>
@@ -2975,16 +2906,16 @@
       <c r="A8" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="E8" s="42" t="n">
+      <c r="E8" s="14" t="n">
         <f aca="false">RADIANS(B8)</f>
         <v>0.0174532925199433</v>
       </c>
@@ -2993,34 +2924,34 @@
       <c r="A9" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="43" t="n">
+      <c r="B9" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E9" s="44" t="n">
+      <c r="E9" s="16" t="n">
         <f aca="false">RADIANS(B9)</f>
         <v>0.0174532925199433</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="43" t="n">
+      <c r="B10" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="46" t="n">
+      <c r="E10" s="27" t="n">
         <f aca="false">RADIANS(B10)</f>
         <v>0.0174532925199433</v>
       </c>
@@ -3029,7 +2960,7 @@
       <c r="A11" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="47" t="n">
+      <c r="B11" s="36" t="n">
         <v>0.1</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -3038,7 +2969,7 @@
       <c r="D11" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="E11" s="48" t="n">
+      <c r="E11" s="37" t="n">
         <f aca="false">B11</f>
         <v>0.1</v>
       </c>
@@ -3047,7 +2978,7 @@
       <c r="A12" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="49" t="n">
+      <c r="B12" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -3056,7 +2987,7 @@
       <c r="D12" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E12" s="50" t="n">
+      <c r="E12" s="38" t="n">
         <f aca="false">B12</f>
         <v>0.1</v>
       </c>
@@ -3065,16 +2996,16 @@
       <c r="A13" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="49" t="n">
+      <c r="B13" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="51" t="n">
+      <c r="E13" s="39" t="n">
         <f aca="false">B13</f>
         <v>0.1</v>
       </c>
@@ -3083,16 +3014,16 @@
       <c r="A14" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B14" s="33" t="n">
+      <c r="B14" s="29" t="n">
         <v>1737</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="52" t="n">
+      <c r="E14" s="40" t="n">
         <f aca="false">B14*1000</f>
         <v>1737000</v>
       </c>
@@ -3101,16 +3032,16 @@
       <c r="A15" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B15" s="36" t="n">
+      <c r="B15" s="31" t="n">
         <v>0.001</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E15" s="53" t="n">
+      <c r="E15" s="41" t="n">
         <f aca="false">B15*1000</f>
         <v>1</v>
       </c>
@@ -3119,16 +3050,16 @@
       <c r="A16" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B16" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="37" t="s">
+      <c r="B16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="E16" s="54" t="n">
+      <c r="E16" s="42" t="n">
         <f aca="false">B16*1000</f>
         <v>0</v>
       </c>
@@ -3137,16 +3068,16 @@
       <c r="A17" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B17" s="33" t="n">
+      <c r="B17" s="29" t="n">
         <v>1737</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="E17" s="52" t="n">
+      <c r="E17" s="40" t="n">
         <f aca="false">B17*1000</f>
         <v>1737000</v>
       </c>
@@ -3155,16 +3086,16 @@
       <c r="A18" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B18" s="36" t="n">
+      <c r="B18" s="31" t="n">
         <v>0</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E18" s="53" t="n">
+      <c r="E18" s="41" t="n">
         <f aca="false">B18*1000</f>
         <v>0</v>
       </c>
@@ -3173,16 +3104,16 @@
       <c r="A19" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="38" t="n">
+      <c r="B19" s="32" t="n">
         <v>0.001</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="E19" s="54" t="n">
+      <c r="E19" s="42" t="n">
         <f aca="false">B19*1000</f>
         <v>1</v>
       </c>
@@ -3191,16 +3122,16 @@
       <c r="A20" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="33" t="n">
+      <c r="B20" s="29" t="n">
         <v>1737</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="E20" s="52" t="n">
+      <c r="E20" s="40" t="n">
         <f aca="false">B20*1000</f>
         <v>1737000</v>
       </c>
@@ -3209,16 +3140,16 @@
       <c r="A21" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B21" s="36" t="n">
+      <c r="B21" s="31" t="n">
         <v>0.001</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E21" s="53" t="n">
+      <c r="E21" s="41" t="n">
         <f aca="false">B21*1000</f>
         <v>1</v>
       </c>
@@ -3227,49 +3158,49 @@
       <c r="A22" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="B22" s="38" t="n">
+      <c r="B22" s="32" t="n">
         <v>0.001</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="54" t="n">
+      <c r="E22" s="42" t="n">
         <f aca="false">B22*1000</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B23" s="35" t="n">
+      <c r="B23" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="55" t="n">
+      <c r="E23" s="41" t="n">
         <f aca="false">B23</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B24" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" s="35" t="s">
+      <c r="B24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="41" t="s">
+      <c r="D24" s="13" t="s">
         <v>153</v>
       </c>
       <c r="E24" s="8" t="n">
@@ -3278,37 +3209,37 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B25" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="35" t="s">
+      <c r="B25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D25" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="E25" s="55" t="n">
+      <c r="E25" s="41" t="n">
         <f aca="false">B25/3</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="35" t="s">
+      <c r="B26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="41" t="s">
+      <c r="D26" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="E26" s="55" t="n">
+      <c r="E26" s="41" t="n">
         <f aca="false">B26/3</f>
         <v>0</v>
       </c>
@@ -3332,7 +3263,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="A39:E41 A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3599,7 +3530,7 @@
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A39:E41 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4789,13 +4720,13 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A39:E41 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="56" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="43" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="14.71"/>
@@ -4804,55 +4735,55 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="58" t="s">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="47" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="62" t="n">
+      <c r="B2" s="17" t="n">
         <f aca="false">0.00000016*3</f>
         <v>4.8E-007</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="7" t="s">
         <v>174</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="E2" s="44" t="n">
+      <c r="E2" s="16" t="n">
         <f aca="false">B2/3</f>
         <v>1.6E-007</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="63" t="n">
+      <c r="B3" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E3" s="44" t="n">
+      <c r="E3" s="16" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
@@ -4862,25 +4793,25 @@
       <c r="A4" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="B4" s="64" t="n">
+      <c r="B4" s="48" t="n">
         <v>0.05</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="E4" s="46" t="n">
+      <c r="E4" s="27" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
         <v>4.84813681109536E-006</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="63" t="n">
+      <c r="B5" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -4889,16 +4820,16 @@
       <c r="D5" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="E5" s="44" t="n">
+      <c r="E5" s="16" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="63" t="n">
+      <c r="B6" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -4907,7 +4838,7 @@
       <c r="D6" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E6" s="44" t="n">
+      <c r="E6" s="16" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
@@ -4916,7 +4847,7 @@
       <c r="A7" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B7" s="63" t="n">
+      <c r="B7" s="18" t="n">
         <v>1.5</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -4925,7 +4856,7 @@
       <c r="D7" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="E7" s="44" t="n">
+      <c r="E7" s="16" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
@@ -4934,7 +4865,7 @@
       <c r="A8" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B8" s="63" t="n">
+      <c r="B8" s="18" t="n">
         <v>1.5</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -4943,7 +4874,7 @@
       <c r="D8" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="E8" s="44" t="n">
+      <c r="E8" s="16" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
@@ -4952,7 +4883,7 @@
       <c r="A9" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B9" s="63" t="n">
+      <c r="B9" s="18" t="n">
         <v>9</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -4961,7 +4892,7 @@
       <c r="D9" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="E9" s="44" t="n">
+      <c r="E9" s="16" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
         <v>1.45444104332861E-005</v>
       </c>
@@ -4970,7 +4901,7 @@
       <c r="A10" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B10" s="40" t="n">
+      <c r="B10" s="34" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -4979,16 +4910,16 @@
       <c r="D10" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="42" t="n">
+      <c r="E10" s="14" t="n">
         <f aca="false">B10/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="65" t="n">
+      <c r="B11" s="49" t="n">
         <v>3</v>
       </c>
       <c r="C11" s="26" t="s">
@@ -4997,7 +4928,7 @@
       <c r="D11" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="E11" s="46" t="n">
+      <c r="E11" s="27" t="n">
         <f aca="false">B11/3</f>
         <v>1</v>
       </c>
@@ -5006,7 +4937,7 @@
       <c r="A12" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="56" t="n">
+      <c r="B12" s="43" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -5024,7 +4955,7 @@
       <c r="A13" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B13" s="56" t="n">
+      <c r="B13" s="43" t="n">
         <v>100</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -5042,7 +4973,7 @@
       <c r="A14" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B14" s="56" t="n">
+      <c r="B14" s="43" t="n">
         <v>10</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -5075,213 +5006,213 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A39:E41 B19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="35" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="51.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="66" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="35" width="17.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="35" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="7" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="51.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="50" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="17.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="7" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="41" t="n">
+      <c r="B2" s="13" t="n">
         <v>4000</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="E2" s="42" t="n">
+      <c r="E2" s="14" t="n">
         <f aca="false">B2/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B3" s="35" t="n">
+      <c r="B3" s="7" t="n">
         <v>4000</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="E3" s="44" t="n">
+      <c r="E3" s="16" t="n">
         <f aca="false">B3/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B4" s="35" t="n">
+      <c r="B4" s="7" t="n">
         <v>4000</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="E4" s="44" t="n">
+      <c r="E4" s="16" t="n">
         <f aca="false">B4/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B5" s="35" t="n">
+      <c r="B5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E5" s="44" t="n">
+      <c r="E5" s="16" t="n">
         <f aca="false">B5/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B6" s="35" t="n">
+      <c r="B6" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E6" s="44" t="n">
+      <c r="E6" s="16" t="n">
         <f aca="false">B6/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B7" s="35" t="n">
+      <c r="B7" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E7" s="44" t="n">
+      <c r="E7" s="16" t="n">
         <f aca="false">B7/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="35" t="n">
+      <c r="B8" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="E8" s="44" t="n">
+      <c r="E8" s="16" t="n">
         <f aca="false">B8/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B9" s="35" t="n">
+      <c r="B9" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="E9" s="44" t="n">
+      <c r="E9" s="16" t="n">
         <f aca="false">B9/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="B10" s="35" t="n">
+      <c r="B10" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="E10" s="44" t="n">
+      <c r="E10" s="16" t="n">
         <f aca="false">B10/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B11" s="35" t="n">
+      <c r="B11" s="7" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="7" t="s">
         <v>188</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E11" s="44" t="n">
+      <c r="E11" s="16" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
@@ -5290,17 +5221,17 @@
       <c r="A12" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B12" s="35" t="n">
+      <c r="B12" s="7" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="7" t="s">
         <v>188</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E12" s="44" t="n">
+      <c r="E12" s="16" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
@@ -5309,17 +5240,17 @@
       <c r="A13" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="B13" s="35" t="n">
+      <c r="B13" s="7" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="7" t="s">
         <v>188</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E13" s="44" t="n">
+      <c r="E13" s="16" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
@@ -5328,17 +5259,17 @@
       <c r="A14" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B14" s="35" t="n">
+      <c r="B14" s="7" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="7" t="s">
         <v>188</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E14" s="44" t="n">
+      <c r="E14" s="16" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
@@ -5347,17 +5278,17 @@
       <c r="A15" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B15" s="35" t="n">
+      <c r="B15" s="7" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="7" t="s">
         <v>188</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E15" s="44" t="n">
+      <c r="E15" s="16" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
@@ -5366,55 +5297,55 @@
       <c r="A16" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B16" s="35" t="n">
+      <c r="B16" s="7" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="7" t="s">
         <v>188</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E16" s="44" t="n">
+      <c r="E16" s="16" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B17" s="35" t="n">
+      <c r="B17" s="7" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E17" s="44" t="n">
+      <c r="E17" s="16" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="B18" s="35" t="n">
+      <c r="B18" s="7" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E18" s="44" t="n">
+      <c r="E18" s="16" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
@@ -5423,17 +5354,17 @@
       <c r="A19" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="B19" s="37" t="n">
+      <c r="B19" s="26" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C19" s="68" t="s">
+      <c r="C19" s="51" t="s">
         <v>177</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="E19" s="46" t="n">
+      <c r="E19" s="27" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
@@ -5457,47 +5388,47 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A39:E41 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="43" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="35" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="66" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="35" width="25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="35" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="50" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="7" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="58" t="s">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="47" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="str">
+      <c r="A2" s="5" t="str">
         <f aca="false">truthStateParams!A2</f>
         <v>Q_grav</v>
       </c>
-      <c r="B2" s="62" t="n">
+      <c r="B2" s="17" t="n">
         <f aca="false">truthStateParams!B2</f>
         <v>4.8E-007</v>
       </c>
-      <c r="C2" s="35" t="str">
+      <c r="C2" s="7" t="str">
         <f aca="false">truthStateParams!C2</f>
         <v>m^2/s^3</v>
       </c>
@@ -5505,64 +5436,64 @@
         <f aca="false">truthStateParams!D2</f>
         <v>3-sigma non-gravitational process noise</v>
       </c>
-      <c r="E2" s="44" t="n">
+      <c r="E2" s="16" t="n">
         <f aca="false">B2/3</f>
         <v>1.6E-007</v>
       </c>
-      <c r="F2" s="66"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="61" t="str">
+      <c r="A3" s="5" t="str">
         <f aca="false">truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
       </c>
-      <c r="B3" s="63" t="n">
+      <c r="B3" s="18" t="n">
         <f aca="false">truthStateParams!B3</f>
         <v>5</v>
       </c>
-      <c r="C3" s="62" t="str">
+      <c r="C3" s="17" t="str">
         <f aca="false">truthStateParams!C3</f>
         <v>deg/hr</v>
       </c>
-      <c r="D3" s="35" t="str">
+      <c r="D3" s="7" t="str">
         <f aca="false">truthStateParams!D3</f>
         <v>3-sigma steady-state gyro bias</v>
       </c>
-      <c r="E3" s="44" t="n">
+      <c r="E3" s="16" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
-      <c r="F3" s="66"/>
+      <c r="F3" s="50"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="str">
         <f aca="false">truthStateParams!A4</f>
         <v>arw</v>
       </c>
-      <c r="B4" s="64" t="n">
+      <c r="B4" s="48" t="n">
         <f aca="false">truthStateParams!B4</f>
         <v>0.05</v>
       </c>
-      <c r="C4" s="37" t="str">
+      <c r="C4" s="26" t="str">
         <f aca="false">truthStateParams!C4</f>
         <v>deg/sqrt(hr)</v>
       </c>
-      <c r="D4" s="37" t="str">
+      <c r="D4" s="26" t="str">
         <f aca="false">truthStateParams!D4</f>
         <v>3-sigma angular random walk</v>
       </c>
-      <c r="E4" s="46" t="n">
+      <c r="E4" s="27" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
         <v>4.84813681109536E-006</v>
       </c>
-      <c r="F4" s="66"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="61" t="str">
+      <c r="A5" s="5" t="str">
         <f aca="false">truthStateParams!A5</f>
         <v>sig_st_ss</v>
       </c>
-      <c r="B5" s="63" t="n">
+      <c r="B5" s="18" t="n">
         <f aca="false">truthStateParams!B5</f>
         <v>20</v>
       </c>
@@ -5574,18 +5505,18 @@
         <f aca="false">truthStateParams!D5</f>
         <v>3-sigma steady-state star camera misalignment</v>
       </c>
-      <c r="E5" s="44" t="n">
+      <c r="E5" s="16" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
-      <c r="F5" s="66"/>
+      <c r="F5" s="50"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="str">
+      <c r="A6" s="5" t="str">
         <f aca="false">truthStateParams!A6</f>
         <v>sig_c_ss</v>
       </c>
-      <c r="B6" s="63" t="n">
+      <c r="B6" s="18" t="n">
         <f aca="false">truthStateParams!B6</f>
         <v>20</v>
       </c>
@@ -5597,7 +5528,7 @@
         <f aca="false">truthStateParams!D6</f>
         <v>3-sigma steady-state terrain camera misalignment</v>
       </c>
-      <c r="E6" s="44" t="n">
+      <c r="E6" s="16" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
@@ -5607,7 +5538,7 @@
         <f aca="false">truthStateParams!A7</f>
         <v>sig_meas_stx</v>
       </c>
-      <c r="B7" s="63" t="n">
+      <c r="B7" s="18" t="n">
         <f aca="false">truthStateParams!B7</f>
         <v>1.5</v>
       </c>
@@ -5619,7 +5550,7 @@
         <f aca="false">truthStateParams!D7</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E7" s="44" t="n">
+      <c r="E7" s="16" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
@@ -5629,7 +5560,7 @@
         <f aca="false">truthStateParams!A8</f>
         <v>sig_meas_sty</v>
       </c>
-      <c r="B8" s="63" t="n">
+      <c r="B8" s="18" t="n">
         <f aca="false">truthStateParams!B8</f>
         <v>1.5</v>
       </c>
@@ -5641,7 +5572,7 @@
         <f aca="false">truthStateParams!D8</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E8" s="44" t="n">
+      <c r="E8" s="16" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
@@ -5651,7 +5582,7 @@
         <f aca="false">truthStateParams!A9</f>
         <v>sig_meas_stz</v>
       </c>
-      <c r="B9" s="63" t="n">
+      <c r="B9" s="18" t="n">
         <f aca="false">truthStateParams!B9</f>
         <v>9</v>
       </c>
@@ -5663,7 +5594,7 @@
         <f aca="false">truthStateParams!D9</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E9" s="44" t="n">
+      <c r="E9" s="16" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
         <v>1.45444104332861E-005</v>
       </c>
@@ -5673,7 +5604,7 @@
         <f aca="false">truthStateParams!A10</f>
         <v>sig_cu</v>
       </c>
-      <c r="B10" s="40" t="n">
+      <c r="B10" s="34" t="n">
         <f aca="false">truthStateParams!B10</f>
         <v>3</v>
       </c>
@@ -5685,17 +5616,17 @@
         <f aca="false">truthStateParams!D10</f>
         <v>3-sigma u component of pixel noise</v>
       </c>
-      <c r="E10" s="42" t="n">
+      <c r="E10" s="14" t="n">
         <f aca="false">B10/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="45" t="str">
+      <c r="A11" s="24" t="str">
         <f aca="false">truthStateParams!A11</f>
         <v>sig_cv</v>
       </c>
-      <c r="B11" s="65" t="n">
+      <c r="B11" s="49" t="n">
         <f aca="false">truthStateParams!B11</f>
         <v>3</v>
       </c>
@@ -5707,17 +5638,17 @@
         <f aca="false">truthStateParams!D11</f>
         <v>3-sigma v component of pixel noise</v>
       </c>
-      <c r="E11" s="46" t="n">
+      <c r="E11" s="27" t="n">
         <f aca="false">B11/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="45" t="str">
+      <c r="A12" s="24" t="str">
         <f aca="false">truthStateParams!A12</f>
         <v>sig_idpos</v>
       </c>
-      <c r="B12" s="65" t="n">
+      <c r="B12" s="49" t="n">
         <f aca="false">truthStateParams!B12</f>
         <v>10</v>
       </c>
@@ -5729,17 +5660,17 @@
         <f aca="false">truthStateParams!D12</f>
         <v>3-sigma change in inertial position measurement uncertainty</v>
       </c>
-      <c r="E12" s="46" t="n">
+      <c r="E12" s="27" t="n">
         <f aca="false">B12/3</f>
         <v>3.33333333333333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="45" t="str">
+      <c r="A13" s="24" t="str">
         <f aca="false">truthStateParams!A13</f>
         <v>sig_loss</v>
       </c>
-      <c r="B13" s="65" t="n">
+      <c r="B13" s="49" t="n">
         <f aca="false">truthStateParams!B13</f>
         <v>100</v>
       </c>
@@ -5751,17 +5682,17 @@
         <f aca="false">truthStateParams!D13</f>
         <v>3-sigma LOSS feature location uncertainty</v>
       </c>
-      <c r="E13" s="46" t="n">
+      <c r="E13" s="27" t="n">
         <f aca="false">B13/3</f>
         <v>33.3333333333333</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="45" t="str">
+      <c r="A14" s="24" t="str">
         <f aca="false">truthStateParams!A14</f>
         <v>sig_mdpos</v>
       </c>
-      <c r="B14" s="65" t="n">
+      <c r="B14" s="49" t="n">
         <f aca="false">truthStateParams!B14</f>
         <v>10</v>
       </c>
@@ -5773,7 +5704,7 @@
         <f aca="false">truthStateParams!D14</f>
         <v>3-sigma change in lunar-referenced position measurement uncertainty</v>
       </c>
-      <c r="E14" s="46" t="n">
+      <c r="E14" s="27" t="n">
         <f aca="false">B14/3</f>
         <v>3.33333333333333</v>
       </c>
@@ -5797,410 +5728,410 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A39:E41 B19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="35" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="51.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="66" width="13.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="35" width="14.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="35" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="7" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="51.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="50" width="13.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="14.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="7" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="69" t="s">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="str">
+      <c r="A2" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
       </c>
-      <c r="B2" s="35" t="n">
+      <c r="B2" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B2</f>
         <v>4000</v>
       </c>
-      <c r="C2" s="35" t="str">
+      <c r="C2" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C2</f>
         <v>m</v>
       </c>
-      <c r="D2" s="35" t="str">
+      <c r="D2" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D2</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E2" s="53" t="n">
+      <c r="E2" s="41" t="n">
         <f aca="false">B2/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F2" s="66"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="61" t="str">
+      <c r="A3" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
       </c>
-      <c r="B3" s="35" t="n">
+      <c r="B3" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B3</f>
         <v>4000</v>
       </c>
-      <c r="C3" s="35" t="str">
+      <c r="C3" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C3</f>
         <v>m</v>
       </c>
-      <c r="D3" s="35" t="str">
+      <c r="D3" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D3</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E3" s="53" t="n">
+      <c r="E3" s="41" t="n">
         <f aca="false">B3/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F3" s="66"/>
+      <c r="F3" s="50"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="61" t="str">
+      <c r="A4" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
       </c>
-      <c r="B4" s="35" t="n">
+      <c r="B4" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B4</f>
         <v>4000</v>
       </c>
-      <c r="C4" s="35" t="str">
+      <c r="C4" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C4</f>
         <v>m</v>
       </c>
-      <c r="D4" s="35" t="str">
+      <c r="D4" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D4</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E4" s="53" t="n">
+      <c r="E4" s="41" t="n">
         <f aca="false">B4/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F4" s="66"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="61" t="str">
+      <c r="A5" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
       </c>
-      <c r="B5" s="35" t="n">
+      <c r="B5" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B5</f>
         <v>3</v>
       </c>
-      <c r="C5" s="35" t="str">
+      <c r="C5" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C5</f>
         <v>m/sec</v>
       </c>
-      <c r="D5" s="35" t="str">
+      <c r="D5" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D5</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E5" s="53" t="n">
+      <c r="E5" s="41" t="n">
         <f aca="false">B5/3</f>
         <v>1</v>
       </c>
-      <c r="F5" s="66"/>
+      <c r="F5" s="50"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="str">
+      <c r="A6" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
       </c>
-      <c r="B6" s="35" t="n">
+      <c r="B6" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B6</f>
         <v>3</v>
       </c>
-      <c r="C6" s="35" t="str">
+      <c r="C6" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C6</f>
         <v>m/sec</v>
       </c>
-      <c r="D6" s="35" t="str">
+      <c r="D6" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D6</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E6" s="53" t="n">
+      <c r="E6" s="41" t="n">
         <f aca="false">B6/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="61" t="str">
+      <c r="A7" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
       </c>
-      <c r="B7" s="35" t="n">
+      <c r="B7" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B7</f>
         <v>3</v>
       </c>
-      <c r="C7" s="35" t="str">
+      <c r="C7" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C7</f>
         <v>m/sec</v>
       </c>
-      <c r="D7" s="35" t="str">
+      <c r="D7" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D7</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E7" s="53" t="n">
+      <c r="E7" s="41" t="n">
         <f aca="false">B7/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="61" t="str">
+      <c r="A8" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
       </c>
-      <c r="B8" s="35" t="n">
+      <c r="B8" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B8</f>
         <v>0.0005</v>
       </c>
-      <c r="C8" s="35" t="str">
+      <c r="C8" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C8</f>
         <v>rad</v>
       </c>
-      <c r="D8" s="35" t="str">
+      <c r="D8" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D8</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E8" s="53" t="n">
+      <c r="E8" s="41" t="n">
         <f aca="false">B8/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="61" t="str">
+      <c r="A9" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
       </c>
-      <c r="B9" s="35" t="n">
+      <c r="B9" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B9</f>
         <v>0.0005</v>
       </c>
-      <c r="C9" s="35" t="str">
+      <c r="C9" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C9</f>
         <v>rad</v>
       </c>
-      <c r="D9" s="35" t="str">
+      <c r="D9" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D9</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E9" s="53" t="n">
+      <c r="E9" s="41" t="n">
         <f aca="false">B9/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="str">
+      <c r="A10" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
       </c>
-      <c r="B10" s="35" t="n">
+      <c r="B10" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B10</f>
         <v>0.0005</v>
       </c>
-      <c r="C10" s="35" t="str">
+      <c r="C10" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C10</f>
         <v>rad</v>
       </c>
-      <c r="D10" s="35" t="str">
+      <c r="D10" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D10</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E10" s="53" t="n">
+      <c r="E10" s="41" t="n">
         <f aca="false">B10/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="61" t="str">
+      <c r="A11" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
       </c>
-      <c r="B11" s="35" t="n">
+      <c r="B11" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B11</f>
         <v>20</v>
       </c>
-      <c r="C11" s="35" t="str">
+      <c r="C11" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C11</f>
         <v>arcsec</v>
       </c>
-      <c r="D11" s="35" t="str">
+      <c r="D11" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D11</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E11" s="53" t="n">
+      <c r="E11" s="41" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="61" t="str">
+      <c r="A12" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
       </c>
-      <c r="B12" s="35" t="n">
+      <c r="B12" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B12</f>
         <v>20</v>
       </c>
-      <c r="C12" s="35" t="str">
+      <c r="C12" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C12</f>
         <v>arcsec</v>
       </c>
-      <c r="D12" s="35" t="str">
+      <c r="D12" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D12</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E12" s="53" t="n">
+      <c r="E12" s="41" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="61" t="str">
+      <c r="A13" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
       </c>
-      <c r="B13" s="35" t="n">
+      <c r="B13" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B13</f>
         <v>20</v>
       </c>
-      <c r="C13" s="35" t="str">
+      <c r="C13" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C13</f>
         <v>arcsec</v>
       </c>
-      <c r="D13" s="35" t="str">
+      <c r="D13" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D13</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E13" s="53" t="n">
+      <c r="E13" s="41" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="61" t="str">
+      <c r="A14" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
       </c>
-      <c r="B14" s="35" t="n">
+      <c r="B14" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B14</f>
         <v>20</v>
       </c>
-      <c r="C14" s="35" t="str">
+      <c r="C14" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C14</f>
         <v>arcsec</v>
       </c>
-      <c r="D14" s="35" t="str">
+      <c r="D14" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D14</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E14" s="53" t="n">
+      <c r="E14" s="41" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="61" t="str">
+      <c r="A15" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
       </c>
-      <c r="B15" s="35" t="n">
+      <c r="B15" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B15</f>
         <v>20</v>
       </c>
-      <c r="C15" s="35" t="str">
+      <c r="C15" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C15</f>
         <v>arcsec</v>
       </c>
-      <c r="D15" s="35" t="str">
+      <c r="D15" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D15</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E15" s="53" t="n">
+      <c r="E15" s="41" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="61" t="str">
+      <c r="A16" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
       </c>
-      <c r="B16" s="35" t="n">
+      <c r="B16" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B16</f>
         <v>20</v>
       </c>
-      <c r="C16" s="35" t="str">
+      <c r="C16" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C16</f>
         <v>arcsec</v>
       </c>
-      <c r="D16" s="35" t="str">
+      <c r="D16" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D16</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E16" s="53" t="n">
+      <c r="E16" s="41" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="61" t="str">
+      <c r="A17" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
       </c>
-      <c r="B17" s="35" t="n">
+      <c r="B17" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B17</f>
         <v>5</v>
       </c>
-      <c r="C17" s="35" t="str">
+      <c r="C17" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C17</f>
         <v>deg/hr</v>
       </c>
-      <c r="D17" s="35" t="str">
+      <c r="D17" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D17</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E17" s="53" t="n">
+      <c r="E17" s="41" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="61" t="str">
+      <c r="A18" s="5" t="str">
         <f aca="false">truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
       </c>
-      <c r="B18" s="35" t="n">
+      <c r="B18" s="7" t="n">
         <f aca="false">truthStateInitialUncertainty!B18</f>
         <v>5</v>
       </c>
-      <c r="C18" s="35" t="str">
+      <c r="C18" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!C18</f>
         <v>deg/hr</v>
       </c>
-      <c r="D18" s="35" t="str">
+      <c r="D18" s="7" t="str">
         <f aca="false">truthStateInitialUncertainty!D18</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E18" s="53" t="n">
+      <c r="E18" s="41" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
@@ -6210,19 +6141,19 @@
         <f aca="false">truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
       </c>
-      <c r="B19" s="37" t="n">
+      <c r="B19" s="26" t="n">
         <f aca="false">truthStateInitialUncertainty!B19</f>
         <v>5</v>
       </c>
-      <c r="C19" s="37" t="str">
+      <c r="C19" s="26" t="str">
         <f aca="false">truthStateInitialUncertainty!C19</f>
         <v>deg/hr</v>
       </c>
-      <c r="D19" s="37" t="str">
+      <c r="D19" s="26" t="str">
         <f aca="false">truthStateInitialUncertainty!D19</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E19" s="54" t="n">
+      <c r="E19" s="42" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>

</xml_diff>

<commit_message>
renamed example to cam, created more transformation matrices, syntehize and predict measurement implemented
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="263">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -370,6 +370,24 @@
   </si>
   <si>
     <t xml:space="preserve">Z component of lunar lander rotation axis (inertial frame)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rcbx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X component of camera offset of body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rcby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y component of camera offset of body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rcbz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z component of camera offset of body</t>
   </si>
   <si>
     <t xml:space="preserve">ri_x</t>
@@ -1277,7 +1295,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.49"/>
@@ -1396,7 +1414,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>6</v>
@@ -1406,7 +1424,7 @@
       </c>
       <c r="E7" s="8" t="n">
         <f aca="false">B7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,7 +1513,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B2" s="29" t="n">
         <v>0.1</v>
@@ -1504,7 +1522,7 @@
         <v>55</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E2" s="30" t="n">
         <f aca="false">B2</f>
@@ -1514,7 +1532,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B3" s="29" t="n">
         <v>0.2</v>
@@ -1523,7 +1541,7 @@
         <v>55</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E3" s="30" t="n">
         <f aca="false">B3</f>
@@ -1533,7 +1551,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B4" s="29" t="n">
         <v>0.3</v>
@@ -1542,7 +1560,7 @@
         <v>55</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E4" s="33" t="n">
         <f aca="false">B4</f>
@@ -1552,16 +1570,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B5" s="31" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E5" s="30" t="n">
         <f aca="false">B5</f>
@@ -1571,16 +1589,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B6" s="31" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E6" s="30" t="n">
         <f aca="false">B6</f>
@@ -1590,16 +1608,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B7" s="31" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E7" s="30" t="n">
         <f aca="false">B7</f>
@@ -1609,7 +1627,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B8" s="34" t="n">
         <v>0.1</v>
@@ -1618,7 +1636,7 @@
         <v>68</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E8" s="14" t="n">
         <f aca="false">RADIANS(B8)</f>
@@ -1628,7 +1646,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B9" s="35" t="n">
         <v>0.2</v>
@@ -1637,7 +1655,7 @@
         <v>68</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E9" s="16" t="n">
         <f aca="false">RADIANS(B9)</f>
@@ -1647,7 +1665,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B10" s="35" t="n">
         <v>0.3</v>
@@ -1656,7 +1674,7 @@
         <v>68</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E10" s="27" t="n">
         <f aca="false">RADIANS(B10)</f>
@@ -1666,16 +1684,16 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B11" s="36" t="n">
         <v>0.1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E11" s="37" t="n">
         <f aca="false">B11</f>
@@ -1685,16 +1703,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B12" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E12" s="38" t="n">
         <f aca="false">B12</f>
@@ -1704,16 +1722,16 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B13" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E13" s="39" t="n">
         <f aca="false">B13</f>
@@ -1723,7 +1741,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B14" s="29" t="n">
         <v>0.1</v>
@@ -1732,7 +1750,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E14" s="40" t="n">
         <f aca="false">B14</f>
@@ -1742,7 +1760,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B15" s="29" t="n">
         <v>0.2</v>
@@ -1751,7 +1769,7 @@
         <v>55</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E15" s="41" t="n">
         <f aca="false">B15</f>
@@ -1761,7 +1779,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B16" s="29" t="n">
         <v>0.3</v>
@@ -1770,7 +1788,7 @@
         <v>55</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E16" s="42" t="n">
         <f aca="false">B16</f>
@@ -1780,7 +1798,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B17" s="29" t="n">
         <v>0.1</v>
@@ -1789,7 +1807,7 @@
         <v>55</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E17" s="40" t="n">
         <f aca="false">B17</f>
@@ -1799,7 +1817,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B18" s="29" t="n">
         <v>0.2</v>
@@ -1808,7 +1826,7 @@
         <v>55</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E18" s="41" t="n">
         <f aca="false">B18</f>
@@ -1818,7 +1836,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B19" s="29" t="n">
         <v>0.3</v>
@@ -1827,7 +1845,7 @@
         <v>55</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E19" s="42" t="n">
         <f aca="false">B19</f>
@@ -1837,7 +1855,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B20" s="29" t="n">
         <v>0.1</v>
@@ -1846,7 +1864,7 @@
         <v>55</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E20" s="40" t="n">
         <f aca="false">B20</f>
@@ -1855,7 +1873,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B21" s="29" t="n">
         <v>0.2</v>
@@ -1864,7 +1882,7 @@
         <v>55</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E21" s="41" t="n">
         <f aca="false">B21</f>
@@ -1873,7 +1891,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B22" s="29" t="n">
         <v>0.3</v>
@@ -1882,7 +1900,7 @@
         <v>55</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E22" s="42" t="n">
         <f aca="false">B22</f>
@@ -1920,7 +1938,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>60</v>
@@ -1928,7 +1946,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>60</v>
@@ -1936,7 +1954,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">hr2min*min2sec</f>
@@ -1945,7 +1963,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>9.81</v>
@@ -1953,7 +1971,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>24</v>
@@ -1961,7 +1979,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">180/3.14159</f>
@@ -1984,10 +2002,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2744,8 +2762,58 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0"/>
-      <c r="E42" s="0"/>
+      <c r="A42" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <f aca="false">B42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <f aca="false">B43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">B44</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2796,7 +2864,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B2" s="29" t="n">
         <v>1737</v>
@@ -2805,7 +2873,7 @@
         <v>43</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E2" s="30" t="n">
         <f aca="false">B2*1000</f>
@@ -2814,7 +2882,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B3" s="31" t="n">
         <v>0</v>
@@ -2823,7 +2891,7 @@
         <v>43</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E3" s="30" t="n">
         <f aca="false">B3*1000</f>
@@ -2832,7 +2900,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B4" s="32" t="n">
         <v>0</v>
@@ -2841,7 +2909,7 @@
         <v>43</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E4" s="33" t="n">
         <f aca="false">B4*1000</f>
@@ -2850,16 +2918,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B5" s="31" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="28" t="s">
         <v>118</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>112</v>
       </c>
       <c r="E5" s="30" t="n">
         <f aca="false">B5*1000</f>
@@ -2868,16 +2936,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B6" s="31" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E6" s="30" t="n">
         <f aca="false">B6*1000</f>
@@ -2886,16 +2954,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B7" s="31" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E7" s="30" t="n">
         <f aca="false">B7*1000</f>
@@ -2904,7 +2972,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B8" s="34" t="n">
         <v>1</v>
@@ -2913,7 +2981,7 @@
         <v>68</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E8" s="14" t="n">
         <f aca="false">RADIANS(B8)</f>
@@ -2922,7 +2990,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B9" s="35" t="n">
         <v>1</v>
@@ -2931,7 +2999,7 @@
         <v>68</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E9" s="16" t="n">
         <f aca="false">RADIANS(B9)</f>
@@ -2940,7 +3008,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="24" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B10" s="35" t="n">
         <v>1</v>
@@ -2949,7 +3017,7 @@
         <v>68</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E10" s="27" t="n">
         <f aca="false">RADIANS(B10)</f>
@@ -2958,16 +3026,16 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B11" s="36" t="n">
         <v>0.1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E11" s="37" t="n">
         <f aca="false">B11</f>
@@ -2976,16 +3044,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B12" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E12" s="38" t="n">
         <f aca="false">B12</f>
@@ -2994,16 +3062,16 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B13" s="31" t="n">
         <v>0.1</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E13" s="39" t="n">
         <f aca="false">B13</f>
@@ -3012,7 +3080,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B14" s="29" t="n">
         <v>1737</v>
@@ -3021,7 +3089,7 @@
         <v>43</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E14" s="40" t="n">
         <f aca="false">B14*1000</f>
@@ -3030,7 +3098,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B15" s="31" t="n">
         <v>0.001</v>
@@ -3039,7 +3107,7 @@
         <v>43</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E15" s="41" t="n">
         <f aca="false">B15*1000</f>
@@ -3048,7 +3116,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B16" s="32" t="n">
         <v>0</v>
@@ -3057,7 +3125,7 @@
         <v>43</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E16" s="42" t="n">
         <f aca="false">B16*1000</f>
@@ -3066,7 +3134,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B17" s="29" t="n">
         <v>1737</v>
@@ -3075,7 +3143,7 @@
         <v>43</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E17" s="40" t="n">
         <f aca="false">B17*1000</f>
@@ -3084,7 +3152,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B18" s="31" t="n">
         <v>0</v>
@@ -3093,7 +3161,7 @@
         <v>43</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E18" s="41" t="n">
         <f aca="false">B18*1000</f>
@@ -3102,7 +3170,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B19" s="32" t="n">
         <v>0.001</v>
@@ -3111,7 +3179,7 @@
         <v>43</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E19" s="42" t="n">
         <f aca="false">B19*1000</f>
@@ -3120,7 +3188,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B20" s="29" t="n">
         <v>1737</v>
@@ -3129,7 +3197,7 @@
         <v>43</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E20" s="40" t="n">
         <f aca="false">B20*1000</f>
@@ -3138,7 +3206,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B21" s="31" t="n">
         <v>0.001</v>
@@ -3147,7 +3215,7 @@
         <v>43</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E21" s="41" t="n">
         <f aca="false">B21*1000</f>
@@ -3156,7 +3224,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B22" s="32" t="n">
         <v>0.001</v>
@@ -3165,7 +3233,7 @@
         <v>43</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E22" s="42" t="n">
         <f aca="false">B22*1000</f>
@@ -3174,7 +3242,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B23" s="7" t="n">
         <v>1</v>
@@ -3183,7 +3251,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E23" s="41" t="n">
         <f aca="false">B23</f>
@@ -3192,7 +3260,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>0</v>
@@ -3201,7 +3269,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E24" s="8" t="n">
         <f aca="false">B24/3</f>
@@ -3210,7 +3278,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B25" s="7" t="n">
         <v>0</v>
@@ -3219,7 +3287,7 @@
         <v>6</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E25" s="41" t="n">
         <f aca="false">B25/3</f>
@@ -3228,7 +3296,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B26" s="7" t="n">
         <v>0</v>
@@ -3237,7 +3305,7 @@
         <v>6</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E26" s="41" t="n">
         <f aca="false">B26/3</f>
@@ -3276,24 +3344,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -3310,7 +3378,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
@@ -3327,7 +3395,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>7</v>
@@ -3344,7 +3412,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>10</v>
@@ -3361,7 +3429,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>13</v>
@@ -3378,7 +3446,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>16</v>
@@ -3395,7 +3463,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>19</v>
@@ -3412,7 +3480,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>22</v>
@@ -3429,7 +3497,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B2</f>
@@ -3471,7 +3539,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">B9</f>
@@ -3492,7 +3560,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">B2</f>
@@ -3543,24 +3611,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -3577,7 +3645,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
@@ -3594,7 +3662,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>7</v>
@@ -3611,7 +3679,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>10</v>
@@ -3628,7 +3696,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>13</v>
@@ -3645,7 +3713,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>16</v>
@@ -3662,7 +3730,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>19</v>
@@ -3679,7 +3747,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B2</f>
@@ -3721,7 +3789,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B2</f>
@@ -4753,17 +4821,17 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B2" s="17" t="n">
         <f aca="false">0.00000016*3</f>
         <v>4.8E-007</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="E2" s="16" t="n">
         <f aca="false">B2/3</f>
@@ -4772,16 +4840,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B3" s="18" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="E3" s="16" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
@@ -4791,16 +4859,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B4" s="48" t="n">
         <v>0.05</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="E4" s="27" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
@@ -4809,16 +4877,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B5" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="E5" s="16" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
@@ -4827,16 +4895,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B6" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="E6" s="16" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
@@ -4845,16 +4913,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B7" s="18" t="n">
         <v>1.5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E7" s="16" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
@@ -4863,16 +4931,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B8" s="18" t="n">
         <v>1.5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E8" s="16" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
@@ -4881,16 +4949,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B9" s="18" t="n">
         <v>9</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E9" s="16" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
@@ -4899,16 +4967,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B10" s="34" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E10" s="14" t="n">
         <f aca="false">B10/3</f>
@@ -4917,16 +4985,16 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B11" s="49" t="n">
         <v>3</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="E11" s="27" t="n">
         <f aca="false">B11/3</f>
@@ -4935,7 +5003,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B12" s="43" t="n">
         <v>10</v>
@@ -4944,7 +5012,7 @@
         <v>55</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E12" s="10" t="n">
         <f aca="false">B12/3</f>
@@ -4953,7 +5021,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B13" s="43" t="n">
         <v>100</v>
@@ -4962,7 +5030,7 @@
         <v>55</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="E13" s="10" t="n">
         <f aca="false">B13/3</f>
@@ -4971,7 +5039,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B14" s="43" t="n">
         <v>10</v>
@@ -4980,7 +5048,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="E14" s="10" t="n">
         <f aca="false">B14/3</f>
@@ -5038,7 +5106,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B2" s="13" t="n">
         <v>4000</v>
@@ -5047,7 +5115,7 @@
         <v>55</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="E2" s="14" t="n">
         <f aca="false">B2/3</f>
@@ -5056,7 +5124,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>4000</v>
@@ -5065,7 +5133,7 @@
         <v>55</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="E3" s="16" t="n">
         <f aca="false">B3/3</f>
@@ -5074,7 +5142,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>4000</v>
@@ -5083,7 +5151,7 @@
         <v>55</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="E4" s="16" t="n">
         <f aca="false">B4/3</f>
@@ -5092,16 +5160,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="E5" s="16" t="n">
         <f aca="false">B5/3</f>
@@ -5110,16 +5178,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="E6" s="16" t="n">
         <f aca="false">B6/3</f>
@@ -5128,16 +5196,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="E7" s="16" t="n">
         <f aca="false">B7/3</f>
@@ -5146,16 +5214,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>0.0005</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="E8" s="16" t="n">
         <f aca="false">B8/3</f>
@@ -5164,16 +5232,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>0.0005</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="E9" s="16" t="n">
         <f aca="false">B9/3</f>
@@ -5182,16 +5250,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>0.0005</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="E10" s="16" t="n">
         <f aca="false">B10/3</f>
@@ -5200,17 +5268,17 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B11" s="7" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E11" s="16" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
@@ -5219,17 +5287,17 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B12" s="7" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E12" s="16" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
@@ -5238,17 +5306,17 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B13" s="7" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E13" s="16" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
@@ -5257,17 +5325,17 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B14" s="7" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="E14" s="16" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
@@ -5276,17 +5344,17 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B15" s="7" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="E15" s="16" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
@@ -5295,17 +5363,17 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B16" s="7" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="E16" s="16" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
@@ -5314,17 +5382,17 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B17" s="7" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E17" s="16" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
@@ -5333,17 +5401,17 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B18" s="7" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E18" s="16" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
@@ -5352,17 +5420,17 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B19" s="26" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E19" s="27" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>

</xml_diff>

<commit_message>
Plots, fixing weird jump
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1292,7 +1292,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1396,7 +1396,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>6</v>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="E6" s="8" t="n">
         <f aca="false">B6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2005,7 +2005,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2054,7 +2054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
I think its good
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -1295,7 +1295,7 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1484,8 +1484,8 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1577,7 +1577,7 @@
         <v>238</v>
       </c>
       <c r="B5" s="53" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>239</v>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="E5" s="30" t="n">
         <f aca="false">B5</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1596,7 +1596,7 @@
         <v>240</v>
       </c>
       <c r="B6" s="7" t="n">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>239</v>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="E6" s="30" t="n">
         <f aca="false">B6</f>
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1615,7 +1615,7 @@
         <v>241</v>
       </c>
       <c r="B7" s="26" t="n">
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>239</v>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="E7" s="30" t="n">
         <f aca="false">B7</f>
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -2009,7 +2009,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>